<commit_message>
Include tasks activation into the script
</commit_message>
<xml_diff>
--- a/inst/extdata/mean-model-workflow-input.xlsx
+++ b/inst/extdata/mean-model-workflow-input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\R-RE-tests\Workflow Srcipts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="830" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" tabRatio="830"/>
   </bookViews>
   <sheets>
     <sheet name="MeanModelSimulation" sheetId="3" r:id="rId1"/>
@@ -193,14 +193,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="244">
   <si>
     <t>reportName</t>
   </si>
   <si>
-    <t>dataTpFilter</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -219,12 +216,6 @@
     <t>function handle to calculate the PK Parameter, if empty default function, which calculates default OSP Suite PK Parameter is used</t>
   </si>
   <si>
-    <t>TaskdoVPC</t>
-  </si>
-  <si>
-    <t>TaskdoSensitivityAnalysis</t>
-  </si>
-  <si>
     <t>sensitivity analysis is performed</t>
   </si>
   <si>
@@ -238,12 +229,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>default plots will be generated</t>
-  </si>
-  <si>
-    <t>Following entries define tasks, which should be performed for all simulations. Only the entries of the first simulation are taken into account</t>
   </si>
   <si>
     <t>data</t>
@@ -284,16 +269,7 @@
     <t>SensitivityParameter</t>
   </si>
   <si>
-    <t>TaskdoAbsorptionPlots</t>
-  </si>
-  <si>
     <t>absorption is plotted</t>
-  </si>
-  <si>
-    <t>massbalance will be checked</t>
-  </si>
-  <si>
-    <t>TaskcheckMassbalance</t>
   </si>
   <si>
     <t>simulation path ID</t>
@@ -939,6 +915,69 @@
   </si>
   <si>
     <t>path</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tasks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Following entries define tasks, which should be performed for all simulations. Only the entries of the first simulation are taken into account</t>
+    </r>
+  </si>
+  <si>
+    <t>simulate</t>
+  </si>
+  <si>
+    <t>calculatePKParameters</t>
+  </si>
+  <si>
+    <t>calculateSensitivity</t>
+  </si>
+  <si>
+    <t>plotTimeProfilesAndResiduals</t>
+  </si>
+  <si>
+    <t>plotAbsorption</t>
+  </si>
+  <si>
+    <t>plotMassBalance</t>
+  </si>
+  <si>
+    <t>plotSensitivity</t>
+  </si>
+  <si>
+    <t>plotPKParameters</t>
+  </si>
+  <si>
+    <t>PK parameters are calculated</t>
+  </si>
+  <si>
+    <t>tables of PK parameters values are performed</t>
+  </si>
+  <si>
+    <t>default plots for time profiles and residuals are generated</t>
+  </si>
+  <si>
+    <t>plots of sensitivity analysis are performed</t>
+  </si>
+  <si>
+    <t>mass balance is checked</t>
+  </si>
+  <si>
+    <t>time profiles are simulated, if false, simulation results should be already available!</t>
   </si>
 </sst>
 </file>
@@ -1447,11 +1486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ21"/>
+  <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C8" sqref="C8"/>
+      <selection pane="topRight" activeCell="B19" sqref="B19:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1477,58 +1516,58 @@
   <sheetData>
     <row r="1" spans="1:36" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
@@ -1551,13 +1590,13 @@
     </row>
     <row r="2" spans="1:36" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -1596,7 +1635,7 @@
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1635,58 +1674,58 @@
     </row>
     <row r="4" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" t="s">
         <v>150</v>
       </c>
-      <c r="D4" t="s">
+      <c r="L4" t="s">
         <v>151</v>
       </c>
-      <c r="E4" t="s">
+      <c r="M4" t="s">
         <v>152</v>
       </c>
-      <c r="F4" t="s">
+      <c r="N4" t="s">
+        <v>154</v>
+      </c>
+      <c r="O4" t="s">
         <v>153</v>
       </c>
-      <c r="G4" t="s">
-        <v>154</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="P4" t="s">
         <v>155</v>
       </c>
-      <c r="I4" t="s">
+      <c r="Q4" t="s">
+        <v>202</v>
+      </c>
+      <c r="R4" t="s">
         <v>156</v>
-      </c>
-      <c r="J4" t="s">
-        <v>157</v>
-      </c>
-      <c r="K4" t="s">
-        <v>158</v>
-      </c>
-      <c r="L4" t="s">
-        <v>159</v>
-      </c>
-      <c r="M4" t="s">
-        <v>160</v>
-      </c>
-      <c r="N4" t="s">
-        <v>162</v>
-      </c>
-      <c r="O4" t="s">
-        <v>161</v>
-      </c>
-      <c r="P4" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>210</v>
-      </c>
-      <c r="R4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
@@ -1694,117 +1733,117 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5" t="s">
         <v>136</v>
       </c>
-      <c r="D5" t="s">
+      <c r="L5" t="s">
         <v>137</v>
       </c>
-      <c r="E5" t="s">
+      <c r="M5" t="s">
         <v>138</v>
       </c>
-      <c r="F5" t="s">
+      <c r="N5" t="s">
+        <v>154</v>
+      </c>
+      <c r="O5" t="s">
         <v>139</v>
       </c>
-      <c r="G5" t="s">
+      <c r="P5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q5" t="s">
         <v>140</v>
       </c>
-      <c r="H5" t="s">
+      <c r="R5" t="s">
         <v>141</v>
-      </c>
-      <c r="I5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J5" t="s">
-        <v>143</v>
-      </c>
-      <c r="K5" t="s">
-        <v>144</v>
-      </c>
-      <c r="L5" t="s">
-        <v>145</v>
-      </c>
-      <c r="M5" t="s">
-        <v>146</v>
-      </c>
-      <c r="N5" t="s">
-        <v>162</v>
-      </c>
-      <c r="O5" t="s">
-        <v>147</v>
-      </c>
-      <c r="P5" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>148</v>
-      </c>
-      <c r="R5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" t="s">
         <v>165</v>
       </c>
-      <c r="D6" t="s">
+      <c r="L6" t="s">
         <v>166</v>
       </c>
-      <c r="E6" t="s">
+      <c r="M6" t="s">
         <v>167</v>
       </c>
-      <c r="F6" t="s">
+      <c r="N6" t="s">
         <v>168</v>
       </c>
-      <c r="G6" t="s">
+      <c r="O6" t="s">
         <v>169</v>
       </c>
-      <c r="H6" t="s">
+      <c r="P6" t="s">
         <v>170</v>
       </c>
-      <c r="I6" t="s">
+      <c r="Q6" t="s">
         <v>171</v>
       </c>
-      <c r="J6" t="s">
+      <c r="R6" t="s">
         <v>172</v>
-      </c>
-      <c r="K6" t="s">
-        <v>173</v>
-      </c>
-      <c r="L6" t="s">
-        <v>174</v>
-      </c>
-      <c r="M6" t="s">
-        <v>175</v>
-      </c>
-      <c r="N6" t="s">
-        <v>176</v>
-      </c>
-      <c r="O6" t="s">
-        <v>177</v>
-      </c>
-      <c r="P6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>179</v>
-      </c>
-      <c r="R6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1843,72 +1882,72 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="G8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="J8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="K8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="M8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="N8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="O8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="P8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="Q8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="R8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1947,13 +1986,13 @@
     </row>
     <row r="11" spans="1:36" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1991,13 +2030,13 @@
     </row>
     <row r="12" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2035,120 +2074,120 @@
     </row>
     <row r="13" spans="1:36" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>1</v>
+        <v>227</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" t="s">
+        <v>211</v>
+      </c>
+      <c r="I13" t="s">
+        <v>212</v>
+      </c>
+      <c r="J13" t="s">
+        <v>213</v>
+      </c>
+      <c r="K13" t="s">
+        <v>214</v>
+      </c>
+      <c r="L13" t="s">
         <v>215</v>
       </c>
-      <c r="E13" t="s">
+      <c r="M13" t="s">
         <v>216</v>
       </c>
-      <c r="F13" t="s">
+      <c r="N13" t="s">
         <v>217</v>
       </c>
-      <c r="G13" t="s">
+      <c r="O13" t="s">
         <v>218</v>
       </c>
-      <c r="H13" t="s">
+      <c r="P13" t="s">
         <v>219</v>
       </c>
-      <c r="I13" t="s">
+      <c r="Q13" t="s">
         <v>220</v>
       </c>
-      <c r="J13" t="s">
+      <c r="R13" t="s">
         <v>221</v>
-      </c>
-      <c r="K13" t="s">
-        <v>222</v>
-      </c>
-      <c r="L13" t="s">
-        <v>223</v>
-      </c>
-      <c r="M13" t="s">
-        <v>224</v>
-      </c>
-      <c r="N13" t="s">
-        <v>225</v>
-      </c>
-      <c r="O13" t="s">
-        <v>226</v>
-      </c>
-      <c r="P13" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>228</v>
-      </c>
-      <c r="R13" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" t="s">
+        <v>180</v>
+      </c>
+      <c r="I14" t="s">
+        <v>181</v>
+      </c>
+      <c r="J14" t="s">
+        <v>182</v>
+      </c>
+      <c r="K14" t="s">
         <v>183</v>
       </c>
-      <c r="D14" t="s">
+      <c r="L14" t="s">
         <v>184</v>
       </c>
-      <c r="E14" t="s">
+      <c r="M14" t="s">
         <v>185</v>
       </c>
-      <c r="F14" t="s">
+      <c r="N14" t="s">
         <v>186</v>
       </c>
-      <c r="G14" t="s">
+      <c r="O14" t="s">
         <v>187</v>
       </c>
-      <c r="H14" t="s">
+      <c r="P14" t="s">
         <v>188</v>
       </c>
-      <c r="I14" t="s">
+      <c r="Q14" t="s">
         <v>189</v>
       </c>
-      <c r="J14" t="s">
+      <c r="R14" t="s">
         <v>190</v>
-      </c>
-      <c r="K14" t="s">
-        <v>191</v>
-      </c>
-      <c r="L14" t="s">
-        <v>192</v>
-      </c>
-      <c r="M14" t="s">
-        <v>193</v>
-      </c>
-      <c r="N14" t="s">
-        <v>194</v>
-      </c>
-      <c r="O14" t="s">
-        <v>195</v>
-      </c>
-      <c r="P14" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>197</v>
-      </c>
-      <c r="R14" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:36" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2187,13 +2226,13 @@
     </row>
     <row r="16" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -2232,7 +2271,7 @@
     <row r="17" spans="1:36" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>229</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
@@ -2269,12 +2308,12 @@
       <c r="AI17" s="5"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>15</v>
+        <v>230</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2315,10 +2354,10 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>10</v>
+        <v>231</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2359,24 +2398,68 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>29</v>
+        <v>232</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>32</v>
+        <v>233</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>31</v>
+        <v>240</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2403,33 +2486,33 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D2" s="15"/>
     </row>
@@ -2438,49 +2521,49 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2489,120 +2572,120 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>57</v>
-      </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2610,43 +2693,43 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2654,10 +2737,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2673,7 +2756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2684,33 +2767,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -2720,49 +2803,49 @@
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2771,252 +2854,252 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -3024,10 +3107,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -3035,10 +3118,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -3046,10 +3129,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -3057,10 +3140,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -3087,26 +3170,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3132,36 +3215,36 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="24"/>
@@ -3170,13 +3253,13 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="24"/>
@@ -3185,16 +3268,16 @@
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
@@ -3202,19 +3285,19 @@
     </row>
     <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="23" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3242,21 +3325,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B2" s="26">
         <v>2</v>
@@ -3265,12 +3348,12 @@
         <v>0.1</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B3" s="26">
         <v>2</v>
@@ -3279,12 +3362,12 @@
         <v>0.1</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B4" s="26">
         <v>2</v>
@@ -3293,12 +3376,12 @@
         <v>0.1</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B5" s="26">
         <v>2</v>
@@ -3307,12 +3390,12 @@
         <v>0.1</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B6" s="26">
         <v>2</v>
@@ -3321,12 +3404,12 @@
         <v>0.1</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B7" s="26">
         <v>2</v>
@@ -3335,12 +3418,12 @@
         <v>0.1</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B8" s="26">
         <v>2</v>
@@ -3349,7 +3432,7 @@
         <v>0.1</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>